<commit_message>
company name similarity matrix
</commit_message>
<xml_diff>
--- a/Testing_data/2_filtered_dataset.xlsx
+++ b/Testing_data/2_filtered_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rusnesileryte/Documents/GitHub/lma-data-pipeline/Testing_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E19D31F-34A9-2D43-B0FE-99C75E0ECE77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B296B38-717F-2340-93D6-AFEAACD246A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{5D19AA18-6576-8644-8C12-E4EC8ECA4C5E}"/>
   </bookViews>
@@ -1886,13 +1886,13 @@
   <dimension ref="A1:AC62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.15">
@@ -6171,7 +6171,7 @@
         <v>321</v>
       </c>
       <c r="B50" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C50" t="s">
         <v>195</v>
@@ -6349,7 +6349,7 @@
         <v>370</v>
       </c>
       <c r="B52" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="C52" t="s">
         <v>98</v>

</xml_diff>